<commit_message>
No change to table
</commit_message>
<xml_diff>
--- a/incident_history/table/raap_incident_table_2018_aug2021.xlsx
+++ b/incident_history/table/raap_incident_table_2018_aug2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tweiglein/Documents/Graduate School/Virginia Tech - Ph.D./IGC IGEP/RAAP/RAAP_transparency_project/incident_history/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A198C4DA-5DAC-C84C-816D-13F5F5FE5BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{678503E9-FBEF-3F49-B476-2B7187205735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="8560" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>